<commit_message>
* Update export excel file function
</commit_message>
<xml_diff>
--- a/export/ExportTestScene2.xlsx
+++ b/export/ExportTestScene2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="51">
   <si>
     <t>MisMatch</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t>Selected</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>Instrument</t>
   </si>
   <si>
     <t>Trade Number</t>
@@ -494,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -510,12 +504,12 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" t="s" s="6">
+      <c r="H1" s="5"/>
+      <c r="I1" t="s" s="6">
         <v>1</v>
       </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -523,13 +517,11 @@
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
+      <c r="S1" s="5"/>
+      <c r="T1" t="s" s="7">
+        <v>2</v>
+      </c>
       <c r="U1" s="5"/>
-      <c r="V1" t="s" s="7">
-        <v>2</v>
-      </c>
-      <c r="W1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" t="s" s="8">
@@ -581,10 +573,10 @@
         <v>18</v>
       </c>
       <c r="Q2" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s" s="8">
         <v>19</v>
-      </c>
-      <c r="R2" t="s" s="8">
-        <v>20</v>
       </c>
       <c r="S2" t="s" s="8">
         <v>20</v>
@@ -595,19 +587,17 @@
       <c r="U2" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="V2" t="s" s="8">
-        <v>23</v>
-      </c>
-      <c r="W2" t="s" s="8">
-        <v>24</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D3" t="s" s="9">
         <v>26</v>
       </c>
@@ -626,19 +616,17 @@
       <c r="I3" t="s" s="9">
         <v>31</v>
       </c>
-      <c r="J3" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s" s="9">
-        <v>33</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D4" t="s" s="9">
         <v>26</v>
       </c>
@@ -649,29 +637,27 @@
         <v>28</v>
       </c>
       <c r="G4" t="s" s="9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I4" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J4" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D5" t="s" s="9">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s" s="9">
         <v>27</v>
@@ -683,26 +669,24 @@
         <v>29</v>
       </c>
       <c r="H5" t="s" s="9">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K5" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B6" t="s" s="9">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D6" t="s" s="9">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s" s="9">
         <v>27</v>
@@ -711,29 +695,27 @@
         <v>28</v>
       </c>
       <c r="G6" t="s" s="9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I6" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J6" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D7" t="s" s="9">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s" s="9">
         <v>27</v>
@@ -745,26 +727,24 @@
         <v>29</v>
       </c>
       <c r="H7" t="s" s="9">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I7" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J7" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K7" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B8" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D8" t="s" s="9">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>27</v>
@@ -773,29 +753,27 @@
         <v>28</v>
       </c>
       <c r="G8" t="s" s="9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I8" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J8" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K8" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s" s="9">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D9" t="s" s="9">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>27</v>
@@ -807,26 +785,24 @@
         <v>29</v>
       </c>
       <c r="H9" t="s" s="9">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I9" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J9" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K9" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B10" t="s" s="9">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D10" t="s" s="9">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s" s="9">
         <v>27</v>
@@ -835,38 +811,36 @@
         <v>28</v>
       </c>
       <c r="G10" t="s" s="9">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I10" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J10" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K10" t="s" s="9">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B11" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D11" t="s" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s" s="9">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s" s="9">
         <v>30</v>
@@ -874,58 +848,54 @@
       <c r="I11" t="s" s="9">
         <v>31</v>
       </c>
-      <c r="J11" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K11" t="s" s="9">
-        <v>33</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B12" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D12" t="s" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s" s="9">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G12" t="s" s="9">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H12" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I12" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J12" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K12" t="s" s="9">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D13" t="s" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s" s="9">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s" s="9">
         <v>42</v>
@@ -934,292 +904,274 @@
         <v>30</v>
       </c>
       <c r="I13" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J13" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K13" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B14" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D14" t="s" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="I14" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="G14" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="H14" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I14" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J14" t="s" s="9">
-        <v>37</v>
-      </c>
       <c r="K14" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="L14" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="M14" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B15" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D15" t="s" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s" s="9">
+        <v>44</v>
+      </c>
+      <c r="H15" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="I15" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J15" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="G15" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="H15" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I15" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J15" t="s" s="9">
-        <v>37</v>
-      </c>
       <c r="K15" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="L15" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="M15" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B16" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D16" t="s" s="9">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H16" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I16" t="s" s="9">
         <v>31</v>
-      </c>
-      <c r="J16" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K16" t="s" s="9">
-        <v>33</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B17" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D17" t="s" s="9">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s" s="9">
         <v>42</v>
       </c>
       <c r="H17" t="s" s="9">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I17" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J17" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K17" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B18" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D18" t="s" s="9">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E18" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s" s="9">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J18" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K18" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B19" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D19" t="s" s="9">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F19" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G19" t="s" s="9">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H19" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I19" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J19" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K19" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B20" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D20" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="H20" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="I20" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s" s="9">
         <v>41</v>
-      </c>
-      <c r="G20" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="H20" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I20" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J20" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K20" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="L20" t="s" s="9">
-        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B21" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D21" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F21" t="s" s="9">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G21" t="s" s="9">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H21" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I21" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="J21" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K21" t="s" s="9">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B22" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D22" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s" s="9">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="G22" t="s" s="9">
         <v>42</v>
@@ -1228,460 +1180,426 @@
         <v>30</v>
       </c>
       <c r="I22" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J22" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K22" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B23" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D23" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="H23" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="I23" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J23" t="s" s="9">
         <v>41</v>
-      </c>
-      <c r="G23" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="H23" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I23" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J23" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K23" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="L23" t="s" s="9">
-        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s" s="9">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D24" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s" s="9">
+        <v>44</v>
+      </c>
+      <c r="H24" t="s" s="9">
+        <v>35</v>
+      </c>
+      <c r="I24" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J24" t="s" s="9">
         <v>41</v>
-      </c>
-      <c r="G24" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="H24" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I24" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J24" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K24" t="s" s="9">
-        <v>33</v>
-      </c>
-      <c r="L24" t="s" s="9">
-        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="C25" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D25" t="s" s="9">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E25" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F25" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H25" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s" s="9">
         <v>31</v>
-      </c>
-      <c r="J25" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K25" t="s" s="9">
-        <v>33</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B26" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D26" t="s" s="9">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E26" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F26" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s" s="9">
         <v>42</v>
       </c>
       <c r="H26" t="s" s="9">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I26" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J26" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K26" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B27" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D27" t="s" s="9">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F27" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G27" t="s" s="9">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H27" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I27" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J27" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K27" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B28" t="s" s="9">
+        <v>48</v>
+      </c>
+      <c r="C28" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D28" t="s" s="9">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E28" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s" s="9">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H28" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I28" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J28" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K28" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B29" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D29" t="s" s="9">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E29" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F29" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G29" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H29" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I29" t="s" s="9">
         <v>31</v>
-      </c>
-      <c r="J29" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K29" t="s" s="9">
-        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D30" t="s" s="9">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F30" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G30" t="s" s="9">
         <v>42</v>
       </c>
       <c r="H30" t="s" s="9">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I30" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J30" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K30" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B31" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D31" t="s" s="9">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F31" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G31" t="s" s="9">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H31" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I31" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J31" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K31" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B32" t="s" s="9">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D32" t="s" s="9">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F32" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G32" t="s" s="9">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H32" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I32" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J32" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K32" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B33" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D33" t="s" s="9">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F33" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G33" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H33" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I33" t="s" s="9">
         <v>31</v>
-      </c>
-      <c r="J33" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K33" t="s" s="9">
-        <v>33</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B34" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="C34" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D34" t="s" s="9">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F34" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G34" t="s" s="9">
         <v>42</v>
       </c>
       <c r="H34" t="s" s="9">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I34" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="J34" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="K34" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B35" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D35" t="s" s="9">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F35" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G35" t="s" s="9">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H35" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I35" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="J35" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K35" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B36" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s" s="9">
+        <v>25</v>
+      </c>
       <c r="D36" t="s" s="9">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E36" t="s" s="9">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F36" t="s" s="9">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="G36" t="s" s="9">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H36" t="s" s="9">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I36" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="J36" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="K36" t="s" s="9">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="K1:U1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:S1"/>
+    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Function export header
</commit_message>
<xml_diff>
--- a/export/ExportTestScene2.xlsx
+++ b/export/ExportTestScene2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="51">
   <si>
     <t>MisMatch</t>
   </si>
@@ -488,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V36"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -516,12 +516,11 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="5"/>
-      <c r="T1" t="s" s="7">
+      <c r="R1" s="5"/>
+      <c r="S1" t="s" s="7">
         <v>2</v>
       </c>
-      <c r="U1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2">
       <c r="A2" t="s" s="8">
@@ -573,18 +572,15 @@
         <v>18</v>
       </c>
       <c r="Q2" t="s" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R2" t="s" s="8">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="S2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="T2" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="U2" t="s" s="8">
         <v>22</v>
       </c>
     </row>
@@ -938,9 +934,6 @@
       <c r="J14" t="s" s="9">
         <v>41</v>
       </c>
-      <c r="K14" t="s" s="9">
-        <v>31</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="9">
@@ -972,9 +965,6 @@
       </c>
       <c r="J15" t="s" s="9">
         <v>41</v>
-      </c>
-      <c r="K15" t="s" s="9">
-        <v>31</v>
       </c>
     </row>
     <row r="16">
@@ -1598,8 +1588,8 @@
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="I1:S1"/>
-    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="I1:R1"/>
+    <mergeCell ref="S1:T1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Update layout format of output file and tag function
* Adapt header with content
* Fix Systematic value.
+ Add function to make Input header and DB column correspond
</commit_message>
<xml_diff>
--- a/export/ExportTestScene2.xlsx
+++ b/export/ExportTestScene2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="57">
   <si>
     <t>MisMatch</t>
   </si>
@@ -86,85 +86,103 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>FUT PTF</t>
+  </si>
+  <si>
+    <t>FUT1</t>
+  </si>
+  <si>
+    <t>12351</t>
+  </si>
+  <si>
+    <t>EQD</t>
+  </si>
+  <si>
+    <t>FUT</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>DELTA</t>
+  </si>
+  <si>
+    <t>GAMMA</t>
+  </si>
+  <si>
+    <t>FUT2</t>
+  </si>
+  <si>
+    <t>12352</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>EQD PTF</t>
+  </si>
+  <si>
+    <t>SEC2</t>
+  </si>
+  <si>
+    <t>12350</t>
+  </si>
+  <si>
+    <t>OPT</t>
+  </si>
+  <si>
+    <t>OTC</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>SEC1</t>
+  </si>
+  <si>
     <t>12345</t>
   </si>
   <si>
-    <t>EQD</t>
-  </si>
-  <si>
-    <t>OPT</t>
-  </si>
-  <si>
-    <t>OTC</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>FUT3</t>
+  </si>
+  <si>
+    <t>12356</t>
+  </si>
+  <si>
+    <t>12353</t>
+  </si>
+  <si>
+    <t>12354</t>
+  </si>
+  <si>
+    <t>12348</t>
+  </si>
+  <si>
+    <t>12357</t>
   </si>
   <si>
     <t>12347</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>12348</t>
-  </si>
-  <si>
-    <t>12350</t>
-  </si>
-  <si>
-    <t>12351</t>
-  </si>
-  <si>
-    <t>FUT</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>MV</t>
-  </si>
-  <si>
-    <t>DELTA</t>
-  </si>
-  <si>
-    <t>GAMMA</t>
-  </si>
-  <si>
-    <t>12352</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>12353</t>
-  </si>
-  <si>
-    <t>12354</t>
-  </si>
-  <si>
-    <t>12356</t>
-  </si>
-  <si>
-    <t>12357</t>
   </si>
 </sst>
 </file>
@@ -612,6 +630,12 @@
       <c r="I3" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J3" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s" s="9">
+        <v>33</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="9">
@@ -633,13 +657,19 @@
         <v>28</v>
       </c>
       <c r="G4" t="s" s="9">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I4" t="s" s="9">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="J4" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K4" t="s" s="9">
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -647,7 +677,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s" s="9">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s" s="9">
         <v>25</v>
@@ -665,9 +695,15 @@
         <v>29</v>
       </c>
       <c r="H5" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="J5" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K5" t="s" s="9">
         <v>33</v>
       </c>
     </row>
@@ -676,7 +712,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s" s="9">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="9">
         <v>25</v>
@@ -691,13 +727,22 @@
         <v>28</v>
       </c>
       <c r="G6" t="s" s="9">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I6" t="s" s="9">
-        <v>33</v>
+        <v>37</v>
+      </c>
+      <c r="J6" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K6" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s" s="9">
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -705,7 +750,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s" s="9">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s" s="9">
         <v>25</v>
@@ -723,10 +768,19 @@
         <v>29</v>
       </c>
       <c r="H7" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K7" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="L7" t="s" s="9">
         <v>35</v>
-      </c>
-      <c r="I7" t="s" s="9">
-        <v>33</v>
       </c>
     </row>
     <row r="8">
@@ -734,13 +788,13 @@
         <v>23</v>
       </c>
       <c r="B8" t="s" s="9">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s" s="9">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s" s="9">
         <v>27</v>
@@ -749,12 +803,18 @@
         <v>28</v>
       </c>
       <c r="G8" t="s" s="9">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H8" t="s" s="9">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s" s="9">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s" s="9">
         <v>33</v>
       </c>
     </row>
@@ -763,13 +823,13 @@
         <v>23</v>
       </c>
       <c r="B9" t="s" s="9">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s" s="9">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s" s="9">
         <v>27</v>
@@ -781,9 +841,15 @@
         <v>29</v>
       </c>
       <c r="H9" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I9" t="s" s="9">
+        <v>36</v>
+      </c>
+      <c r="J9" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s" s="9">
         <v>33</v>
       </c>
     </row>
@@ -792,27 +858,33 @@
         <v>23</v>
       </c>
       <c r="B10" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s" s="9">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="H10" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="I10" t="s" s="9">
         <v>37</v>
       </c>
-      <c r="C10" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s" s="9">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s" s="9">
-        <v>32</v>
-      </c>
-      <c r="H10" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I10" t="s" s="9">
+      <c r="J10" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K10" t="s" s="9">
         <v>33</v>
       </c>
     </row>
@@ -821,28 +893,34 @@
         <v>23</v>
       </c>
       <c r="B11" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s" s="9">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="E11" t="s" s="9">
+        <v>27</v>
+      </c>
+      <c r="F11" t="s" s="9">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s" s="9">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="I11" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="C11" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="G11" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="H11" t="s" s="9">
-        <v>30</v>
-      </c>
-      <c r="I11" t="s" s="9">
-        <v>31</v>
+      <c r="J11" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K11" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="12">
@@ -850,28 +928,34 @@
         <v>23</v>
       </c>
       <c r="B12" t="s" s="9">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s" s="9">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s" s="9">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s" s="9">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G12" t="s" s="9">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I12" t="s" s="9">
-        <v>41</v>
+        <v>31</v>
+      </c>
+      <c r="J12" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K12" t="s" s="9">
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -879,28 +963,34 @@
         <v>23</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s" s="9">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s" s="9">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s" s="9">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s" s="9">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I13" t="s" s="9">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="J13" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K13" t="s" s="9">
+        <v>47</v>
       </c>
     </row>
     <row r="14">
@@ -908,31 +998,34 @@
         <v>23</v>
       </c>
       <c r="B14" t="s" s="9">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s" s="9">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s" s="9">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E14" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s" s="9">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s" s="9">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H14" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I14" t="s" s="9">
         <v>31</v>
       </c>
       <c r="J14" t="s" s="9">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="K14" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -940,31 +1033,34 @@
         <v>23</v>
       </c>
       <c r="B15" t="s" s="9">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s" s="9">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s" s="9">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F15" t="s" s="9">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s" s="9">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I15" t="s" s="9">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s" s="9">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="K15" t="s" s="9">
+        <v>47</v>
       </c>
     </row>
     <row r="16">
@@ -972,57 +1068,69 @@
         <v>23</v>
       </c>
       <c r="B16" t="s" s="9">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s" s="9">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E16" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G16" t="s" s="9">
         <v>29</v>
       </c>
       <c r="H16" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I16" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J16" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K16" t="s" s="9">
+        <v>33</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="9">
         <v>23</v>
       </c>
       <c r="B17" t="s" s="9">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s" s="9">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G17" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H17" t="s" s="9">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I17" t="s" s="9">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="J17" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K17" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="18">
@@ -1030,28 +1138,34 @@
         <v>23</v>
       </c>
       <c r="B18" t="s" s="9">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s" s="9">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F18" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s" s="9">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H18" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I18" t="s" s="9">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="J18" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K18" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -1059,28 +1173,34 @@
         <v>23</v>
       </c>
       <c r="B19" t="s" s="9">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s" s="9">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s" s="9">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G19" t="s" s="9">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H19" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I19" t="s" s="9">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="J19" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K19" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="20">
@@ -1088,16 +1208,16 @@
         <v>23</v>
       </c>
       <c r="B20" t="s" s="9">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D20" t="s" s="9">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s" s="9">
         <v>28</v>
@@ -1106,13 +1226,19 @@
         <v>29</v>
       </c>
       <c r="H20" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I20" t="s" s="9">
         <v>31</v>
       </c>
       <c r="J20" t="s" s="9">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="K20" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="L20" t="s" s="9">
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -1120,28 +1246,34 @@
         <v>23</v>
       </c>
       <c r="B21" t="s" s="9">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D21" t="s" s="9">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s" s="9">
         <v>28</v>
       </c>
       <c r="G21" t="s" s="9">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H21" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I21" t="s" s="9">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="J21" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K21" t="s" s="9">
+        <v>35</v>
       </c>
     </row>
     <row r="22">
@@ -1149,28 +1281,34 @@
         <v>23</v>
       </c>
       <c r="B22" t="s" s="9">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D22" t="s" s="9">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F22" t="s" s="9">
         <v>28</v>
       </c>
       <c r="G22" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H22" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I22" t="s" s="9">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="J22" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K22" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="23">
@@ -1178,31 +1316,37 @@
         <v>23</v>
       </c>
       <c r="B23" t="s" s="9">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D23" t="s" s="9">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s" s="9">
         <v>28</v>
       </c>
       <c r="G23" t="s" s="9">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H23" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="I23" t="s" s="9">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K23" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="L23" t="s" s="9">
         <v>35</v>
-      </c>
-      <c r="I23" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J23" t="s" s="9">
-        <v>41</v>
       </c>
     </row>
     <row r="24">
@@ -1210,31 +1354,37 @@
         <v>23</v>
       </c>
       <c r="B24" t="s" s="9">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D24" t="s" s="9">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F24" t="s" s="9">
         <v>28</v>
       </c>
       <c r="G24" t="s" s="9">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H24" t="s" s="9">
+        <v>30</v>
+      </c>
+      <c r="I24" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K24" t="s" s="9">
+        <v>33</v>
+      </c>
+      <c r="L24" t="s" s="9">
         <v>35</v>
-      </c>
-      <c r="I24" t="s" s="9">
-        <v>31</v>
-      </c>
-      <c r="J24" t="s" s="9">
-        <v>41</v>
       </c>
     </row>
     <row r="25">
@@ -1242,57 +1392,69 @@
         <v>23</v>
       </c>
       <c r="B25" t="s" s="9">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s" s="9">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E25" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s" s="9">
         <v>29</v>
       </c>
       <c r="H25" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I25" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J25" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K25" t="s" s="9">
+        <v>33</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="9">
         <v>23</v>
       </c>
       <c r="B26" t="s" s="9">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s" s="9">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G26" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H26" t="s" s="9">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s" s="9">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="J26" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K26" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="27">
@@ -1300,28 +1462,34 @@
         <v>23</v>
       </c>
       <c r="B27" t="s" s="9">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D27" t="s" s="9">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E27" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G27" t="s" s="9">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H27" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I27" t="s" s="9">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="J27" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K27" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="28">
@@ -1329,28 +1497,34 @@
         <v>23</v>
       </c>
       <c r="B28" t="s" s="9">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C28" t="s" s="9">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D28" t="s" s="9">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F28" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G28" t="s" s="9">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H28" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I28" t="s" s="9">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="J28" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K28" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="29">
@@ -1358,57 +1532,69 @@
         <v>23</v>
       </c>
       <c r="B29" t="s" s="9">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s" s="9">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s" s="9">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E29" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F29" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="G29" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="G29" t="s" s="9">
-        <v>29</v>
-      </c>
       <c r="H29" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I29" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J29" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K29" t="s" s="9">
+        <v>47</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="9">
         <v>23</v>
       </c>
       <c r="B30" t="s" s="9">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s" s="9">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s" s="9">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E30" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F30" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s" s="9">
         <v>46</v>
-      </c>
-      <c r="G30" t="s" s="9">
-        <v>42</v>
       </c>
       <c r="H30" t="s" s="9">
         <v>30</v>
       </c>
       <c r="I30" t="s" s="9">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="J30" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K30" t="s" s="9">
+        <v>47</v>
       </c>
     </row>
     <row r="31">
@@ -1416,57 +1602,69 @@
         <v>23</v>
       </c>
       <c r="B31" t="s" s="9">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D31" t="s" s="9">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E31" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G31" t="s" s="9">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H31" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I31" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J31" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K31" t="s" s="9">
+        <v>33</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="9">
         <v>23</v>
       </c>
       <c r="B32" t="s" s="9">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D32" t="s" s="9">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F32" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G32" t="s" s="9">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="H32" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I32" t="s" s="9">
-        <v>31</v>
+        <v>36</v>
+      </c>
+      <c r="J32" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K32" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="33">
@@ -1474,28 +1672,34 @@
         <v>23</v>
       </c>
       <c r="B33" t="s" s="9">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D33" t="s" s="9">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F33" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G33" t="s" s="9">
         <v>29</v>
       </c>
       <c r="H33" t="s" s="9">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="I33" t="s" s="9">
-        <v>31</v>
+        <v>37</v>
+      </c>
+      <c r="J33" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K33" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="34">
@@ -1503,28 +1707,34 @@
         <v>23</v>
       </c>
       <c r="B34" t="s" s="9">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s" s="9">
         <v>25</v>
       </c>
       <c r="D34" t="s" s="9">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E34" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s" s="9">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="G34" t="s" s="9">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H34" t="s" s="9">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I34" t="s" s="9">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="J34" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K34" t="s" s="9">
+        <v>33</v>
       </c>
     </row>
     <row r="35">
@@ -1532,57 +1742,69 @@
         <v>23</v>
       </c>
       <c r="B35" t="s" s="9">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s" s="9">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s" s="9">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E35" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F35" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="G35" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="G35" t="s" s="9">
-        <v>43</v>
-      </c>
       <c r="H35" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I35" t="s" s="9">
         <v>31</v>
       </c>
+      <c r="J35" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K35" t="s" s="9">
+        <v>47</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="9">
         <v>23</v>
       </c>
       <c r="B36" t="s" s="9">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s" s="9">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s" s="9">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F36" t="s" s="9">
+        <v>45</v>
+      </c>
+      <c r="G36" t="s" s="9">
         <v>46</v>
       </c>
-      <c r="G36" t="s" s="9">
-        <v>44</v>
-      </c>
       <c r="H36" t="s" s="9">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I36" t="s" s="9">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="J36" t="s" s="9">
+        <v>32</v>
+      </c>
+      <c r="K36" t="s" s="9">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>